<commit_message>
LEGEND: deshielo por uso y export
</commit_message>
<xml_diff>
--- a/data/legend/plantillas/legend_template.xlsx
+++ b/data/legend/plantillas/legend_template.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingmontajes4\Documents\PC-JUAN LOZANO 22032022\WESTON\JUAN LOZANO\TABLA CO2\GITHUB\mi_aplicacion_python\data\legend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingmontajes4\Documents\PC-JUAN LOZANO 22032022\WESTON\JUAN LOZANO\TABLA CO2\GITHUB\mi_aplicacion_python\data\legend\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{225E13A2-E90B-4BB7-850D-C1E88F8C960E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CE95FB-9E29-426E-9B32-EB6CF3159027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8FCE0724-9F65-4FC5-9EC0-BD227B613557}"/>
+    <workbookView xWindow="1440" yWindow="1728" windowWidth="21600" windowHeight="11232" xr2:uid="{8FCE0724-9F65-4FC5-9EC0-BD227B613557}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>ESPECIFICACIONES TECNICAS</t>
   </si>
@@ -87,15 +87,9 @@
     <t>EVAPORADORES</t>
   </si>
   <si>
-    <t>CDS</t>
-  </si>
-  <si>
     <t>LIQUIDA</t>
   </si>
   <si>
-    <t>HG</t>
-  </si>
-  <si>
     <t>DESHIELO</t>
   </si>
   <si>
@@ -103,6 +97,15 @@
   </si>
   <si>
     <t>MODELO</t>
+  </si>
+  <si>
+    <t>LOOP</t>
+  </si>
+  <si>
+    <t>CONTROL</t>
+  </si>
+  <si>
+    <t>DIRECCIÓN</t>
   </si>
 </sst>
 </file>
@@ -112,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0\°&quot;  F&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,12 +144,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -162,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -405,26 +402,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -450,23 +427,95 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -479,81 +528,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -578,22 +552,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>434340</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>85266</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>760717</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>92339</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>279746</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>220433</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{413FD2E0-7AB2-401B-85C8-5428309BB38B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BB07050-E14C-478C-9CB0-0F4885BD1403}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -615,8 +589,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="85266"/>
-          <a:ext cx="3884917" cy="921473"/>
+          <a:off x="434340" y="0"/>
+          <a:ext cx="3807806" cy="967193"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -924,231 +898,261 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE74F0BB-EE57-42E9-8ED7-A2B3DFAABD77}">
-  <dimension ref="A1:P25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAFF4E1B-3766-46AF-AA88-1BA136DF8155}">
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.77734375" style="1" customWidth="1"/>
-    <col min="3" max="16" width="14.77734375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.44140625" style="2"/>
+    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F2" s="3" t="s">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="5"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="9"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F3" s="6" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="6" t="s">
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="6" t="s">
+      <c r="L2" s="26"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="10"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="F4" s="11" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="11" t="s">
+      <c r="H3" s="16"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="11" t="s">
+      <c r="L3" s="16"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="15"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="3"/>
     </row>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F5" s="16" t="s">
+    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="16" t="s">
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="16" t="s">
+      <c r="L4" s="20"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="17"/>
-      <c r="P5" s="22"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="4"/>
     </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
+    <row r="5" spans="1:17" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="23" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="5"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="9"/>
     </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="E7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="25" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="H7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="I7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="3" t="s">
+      <c r="K7" s="7"/>
+      <c r="L7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M8" s="3" t="s">
+      <c r="O7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="Q7" s="9"/>
+    </row>
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="K8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="5"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="31"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D17" s="34"/>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="D18" s="34"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C21" s="34"/>
-    </row>
-    <row r="25" spans="3:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:P9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="I7:P7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="F2:P2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="G1:Q1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="J6:Q6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:Q8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
LEGEND: compresores con multiples modelos
</commit_message>
<xml_diff>
--- a/data/legend/plantillas/legend_template.xlsx
+++ b/data/legend/plantillas/legend_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ingmontajes4\Documents\PC-JUAN LOZANO 22032022\WESTON\JUAN LOZANO\TABLA CO2\GITHUB\mi_aplicacion_python\data\legend\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CE95FB-9E29-426E-9B32-EB6CF3159027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2A1E53-01F4-4E12-9EF5-AE49568F09DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1728" windowWidth="21600" windowHeight="11232" xr2:uid="{8FCE0724-9F65-4FC5-9EC0-BD227B613557}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8FCE0724-9F65-4FC5-9EC0-BD227B613557}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
   <si>
     <t>ESPECIFICACIONES TECNICAS</t>
   </si>
@@ -106,14 +106,141 @@
   </si>
   <si>
     <t>DIRECCIÓN</t>
+  </si>
+  <si>
+    <t>BAJA</t>
+  </si>
+  <si>
+    <t>MEDIA</t>
+  </si>
+  <si>
+    <t>RH</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>CARGA</t>
+  </si>
+  <si>
+    <t>RESERVA %</t>
+  </si>
+  <si>
+    <t>SISTEMA PARALELO</t>
+  </si>
+  <si>
+    <t>COMPRESORES Y ACESORIOS</t>
+  </si>
+  <si>
+    <t>POSICION DE  COMPRESOR EN EL RACK</t>
+  </si>
+  <si>
+    <t>MODELO DE COMPRESOR</t>
+  </si>
+  <si>
+    <t>DEMAND COOLING / CIC</t>
+  </si>
+  <si>
+    <t>VENTILADOR DE CABEZA</t>
+  </si>
+  <si>
+    <t>CONTACTOR</t>
+  </si>
+  <si>
+    <t>BREAKER</t>
+  </si>
+  <si>
+    <t>CONTROL DE CAPACIDAD</t>
+  </si>
+  <si>
+    <t>REGULADOR DE NIVEL DE ACEITE</t>
+  </si>
+  <si>
+    <t>HP NOMINAL</t>
+  </si>
+  <si>
+    <t>REFRIGERANTE</t>
+  </si>
+  <si>
+    <t>TEMPERATURA  DE SUCCIÓN</t>
+  </si>
+  <si>
+    <t>TEMPERATURA DE CONDENSACION</t>
+  </si>
+  <si>
+    <t>CAPACIDAD   BTU/Hr</t>
+  </si>
+  <si>
+    <t>RH   BTU/Hr</t>
+  </si>
+  <si>
+    <t>RLA</t>
+  </si>
+  <si>
+    <t>CONSUMO EN PUNTO DE OPERACIÓN</t>
+  </si>
+  <si>
+    <t>RLA TOTAL</t>
+  </si>
+  <si>
+    <t>CONSUMO TOTAL  PUNTO OPERACIÓN</t>
+  </si>
+  <si>
+    <t>NOTAS:</t>
+  </si>
+  <si>
+    <t>CONDENSADOR</t>
+  </si>
+  <si>
+    <t>WESTON SAS - BOGOTA - COLOMBIA</t>
+  </si>
+  <si>
+    <t>CALCULO</t>
+  </si>
+  <si>
+    <t>REVISO</t>
+  </si>
+  <si>
+    <t>CAPACIDAD</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>VENDEDOR</t>
+  </si>
+  <si>
+    <t>dBA</t>
+  </si>
+  <si>
+    <t>CLIENTE</t>
+  </si>
+  <si>
+    <t>REFR.</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>T. COND</t>
+  </si>
+  <si>
+    <t>DIMENSION</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>ULTIMA REFORMA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0\°&quot;  F&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -145,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,8 +285,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="50">
     <border>
       <left/>
       <right/>
@@ -440,11 +579,367 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -461,31 +956,52 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -500,34 +1016,229 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -899,10 +1610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAFF4E1B-3766-46AF-AA88-1BA136DF8155}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,19 +1629,19 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="9"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="11"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -939,22 +1650,22 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="25" t="s">
+      <c r="H2" s="13"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="25" t="s">
+      <c r="L2" s="13"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="26"/>
+      <c r="P2" s="13"/>
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -964,22 +1675,22 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="15" t="s">
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="15" t="s">
+      <c r="L3" s="23"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="16"/>
+      <c r="P3" s="23"/>
       <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -989,22 +1700,22 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="19" t="s">
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="19" t="s">
+      <c r="L4" s="17"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="20"/>
+      <c r="P4" s="17"/>
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1027,116 +1738,923 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="11" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="9"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="11"/>
     </row>
     <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="6" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="6" t="s">
+      <c r="K7" s="10"/>
+      <c r="L7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="N7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="O7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="6" t="s">
+      <c r="P7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="Q7" s="9"/>
+      <c r="Q7" s="11"/>
     </row>
     <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
       <c r="J8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="K8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="10"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="31"/>
+    </row>
+    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q19" s="35"/>
+    </row>
+    <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="36"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="39"/>
+    </row>
+    <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="41"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="44"/>
+    </row>
+    <row r="22" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" s="46"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="49"/>
+    </row>
+    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+    </row>
+    <row r="24" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="60">
+        <v>1</v>
+      </c>
+      <c r="G26" s="60">
+        <v>2</v>
+      </c>
+      <c r="H26" s="60">
+        <v>3</v>
+      </c>
+      <c r="I26" s="60">
+        <v>4</v>
+      </c>
+      <c r="J26" s="60">
+        <v>5</v>
+      </c>
+      <c r="K26" s="60">
+        <v>6</v>
+      </c>
+      <c r="L26" s="60">
+        <v>7</v>
+      </c>
+      <c r="M26" s="60">
+        <v>8</v>
+      </c>
+      <c r="N26" s="56"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="62"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="65"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="65"/>
+      <c r="L29" s="65"/>
+      <c r="M29" s="65"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="3"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="62"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="65"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="3"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="62"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="65"/>
+      <c r="M31" s="65"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="3"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="65"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="3"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="65"/>
+      <c r="J33" s="65"/>
+      <c r="K33" s="65"/>
+      <c r="L33" s="65"/>
+      <c r="M33" s="65"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="3"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="62"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="65"/>
+      <c r="M34" s="65"/>
+      <c r="N34" s="56"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="3"/>
+    </row>
+    <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="41"/>
+      <c r="L35" s="41"/>
+      <c r="M35" s="41"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="3"/>
+    </row>
+    <row r="36" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="62"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="62"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="67"/>
+      <c r="K36" s="67"/>
+      <c r="L36" s="67"/>
+      <c r="M36" s="67"/>
+      <c r="N36" s="56"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="3"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="68"/>
+      <c r="H37" s="68"/>
+      <c r="I37" s="68"/>
+      <c r="J37" s="68"/>
+      <c r="K37" s="68"/>
+      <c r="L37" s="68"/>
+      <c r="M37" s="68"/>
+      <c r="N37" s="56"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="3"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
+      <c r="K38" s="65"/>
+      <c r="L38" s="65"/>
+      <c r="M38" s="65"/>
+      <c r="N38" s="56"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="3"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A39" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="62"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="65"/>
+      <c r="J39" s="65"/>
+      <c r="K39" s="65"/>
+      <c r="L39" s="65"/>
+      <c r="M39" s="65"/>
+      <c r="N39" s="56"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="3"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A40" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="69"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="69"/>
+      <c r="K40" s="69"/>
+      <c r="L40" s="69"/>
+      <c r="M40" s="69"/>
+      <c r="N40" s="56"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="3"/>
+    </row>
+    <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="62"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="70"/>
+      <c r="J41" s="70"/>
+      <c r="K41" s="70"/>
+      <c r="L41" s="70"/>
+      <c r="M41" s="70"/>
+      <c r="N41" s="56"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="3"/>
+    </row>
+    <row r="42" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="73"/>
+      <c r="N42" s="56"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="3"/>
+    </row>
+    <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="75"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="78"/>
+      <c r="H43" s="78"/>
+      <c r="I43" s="78"/>
+      <c r="J43" s="78"/>
+      <c r="K43" s="78"/>
+      <c r="L43" s="78"/>
+      <c r="M43" s="79"/>
+      <c r="N43" s="80"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="4"/>
+    </row>
+    <row r="44" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+    </row>
+    <row r="45" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="L45" s="11"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="11"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46" s="36"/>
+      <c r="B46" s="82"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="82"/>
+      <c r="G46" s="82"/>
+      <c r="H46" s="82"/>
+      <c r="I46" s="82"/>
+      <c r="J46" s="83"/>
+      <c r="K46" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="L46" s="37"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="85" t="s">
+        <v>56</v>
+      </c>
+      <c r="O46" s="86"/>
+      <c r="P46" s="38"/>
+      <c r="Q46" s="39"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47" s="65"/>
+      <c r="B47" s="87"/>
+      <c r="C47" s="87"/>
+      <c r="D47" s="87"/>
+      <c r="E47" s="87"/>
+      <c r="F47" s="87"/>
+      <c r="G47" s="87"/>
+      <c r="H47" s="87"/>
+      <c r="I47" s="87"/>
+      <c r="J47" s="88"/>
+      <c r="K47" s="89" t="s">
+        <v>22</v>
+      </c>
+      <c r="L47" s="90"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="O47" s="63"/>
+      <c r="P47" s="91"/>
+      <c r="Q47" s="92"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48" s="65"/>
+      <c r="B48" s="87"/>
+      <c r="C48" s="87"/>
+      <c r="D48" s="87"/>
+      <c r="E48" s="87"/>
+      <c r="F48" s="87"/>
+      <c r="G48" s="87"/>
+      <c r="H48" s="87"/>
+      <c r="I48" s="87"/>
+      <c r="J48" s="88"/>
+      <c r="K48" s="89" t="s">
+        <v>58</v>
+      </c>
+      <c r="L48" s="90"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="O48" s="63"/>
+      <c r="P48" s="91"/>
+      <c r="Q48" s="92"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A49" s="65"/>
+      <c r="B49" s="87"/>
+      <c r="C49" s="87"/>
+      <c r="D49" s="87"/>
+      <c r="E49" s="87"/>
+      <c r="F49" s="87"/>
+      <c r="G49" s="87"/>
+      <c r="H49" s="87"/>
+      <c r="I49" s="87"/>
+      <c r="J49" s="88"/>
+      <c r="K49" s="89" t="s">
+        <v>59</v>
+      </c>
+      <c r="L49" s="90"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="O49" s="63"/>
+      <c r="P49" s="91"/>
+      <c r="Q49" s="92"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A50" s="65"/>
+      <c r="B50" s="87"/>
+      <c r="C50" s="87"/>
+      <c r="D50" s="87"/>
+      <c r="E50" s="87"/>
+      <c r="F50" s="87"/>
+      <c r="G50" s="87"/>
+      <c r="H50" s="87"/>
+      <c r="I50" s="87"/>
+      <c r="J50" s="88"/>
+      <c r="K50" s="89" t="s">
+        <v>61</v>
+      </c>
+      <c r="L50" s="90"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="61" t="s">
+        <v>62</v>
+      </c>
+      <c r="O50" s="63"/>
+      <c r="P50" s="91"/>
+      <c r="Q50" s="92"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A51" s="65"/>
+      <c r="B51" s="87"/>
+      <c r="C51" s="87"/>
+      <c r="D51" s="87"/>
+      <c r="E51" s="87"/>
+      <c r="F51" s="87"/>
+      <c r="G51" s="87"/>
+      <c r="H51" s="87"/>
+      <c r="I51" s="87"/>
+      <c r="J51" s="88"/>
+      <c r="K51" s="89" t="s">
+        <v>63</v>
+      </c>
+      <c r="L51" s="90"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="O51" s="63"/>
+      <c r="P51" s="91"/>
+      <c r="Q51" s="92"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A52" s="65"/>
+      <c r="B52" s="87"/>
+      <c r="C52" s="87"/>
+      <c r="D52" s="87"/>
+      <c r="E52" s="87"/>
+      <c r="F52" s="87"/>
+      <c r="G52" s="87"/>
+      <c r="H52" s="87"/>
+      <c r="I52" s="87"/>
+      <c r="J52" s="88"/>
+      <c r="K52" s="89" t="s">
+        <v>65</v>
+      </c>
+      <c r="L52" s="93"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="O52" s="63"/>
+      <c r="P52" s="91"/>
+      <c r="Q52" s="92"/>
+    </row>
+    <row r="53" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="94"/>
+      <c r="B53" s="95"/>
+      <c r="C53" s="95"/>
+      <c r="D53" s="95"/>
+      <c r="E53" s="95"/>
+      <c r="F53" s="95"/>
+      <c r="G53" s="95"/>
+      <c r="H53" s="95"/>
+      <c r="I53" s="95"/>
+      <c r="J53" s="96"/>
+      <c r="K53" s="97" t="s">
+        <v>66</v>
+      </c>
+      <c r="L53" s="98"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="74" t="s">
+        <v>67</v>
+      </c>
+      <c r="O53" s="76"/>
+      <c r="P53" s="99"/>
+      <c r="Q53" s="100"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="G1:Q1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="O3:P3"/>
+  <mergeCells count="79">
+    <mergeCell ref="N51:O51"/>
+    <mergeCell ref="P51:Q51"/>
+    <mergeCell ref="N52:O52"/>
+    <mergeCell ref="P52:Q52"/>
+    <mergeCell ref="N53:O53"/>
+    <mergeCell ref="P53:Q53"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="N49:O49"/>
+    <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="N50:O50"/>
+    <mergeCell ref="P50:Q50"/>
+    <mergeCell ref="N45:Q45"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="F42:M42"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="F43:M43"/>
+    <mergeCell ref="A45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:M25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="A24:M24"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="J6:Q6"/>
     <mergeCell ref="A7:A8"/>
@@ -1153,6 +2671,22 @@
     <mergeCell ref="N7:N8"/>
     <mergeCell ref="O7:O8"/>
     <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="G1:Q1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>